<commit_message>
borde hecho con imagen detras del texto
</commit_message>
<xml_diff>
--- a/databasesandtemplate/basedatos.xlsx
+++ b/databasesandtemplate/basedatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SORACA\Desktop\duro\develop\pdf-generator-with-onlyoffice-docbuilder\databasesandtemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995F9827-F890-4966-8225-323C8D204BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D05B281-AF69-4C19-8A59-1C83BFDD833A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Nombre</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>DNI</t>
+  </si>
+  <si>
+    <t>Efrain</t>
+  </si>
+  <si>
+    <t>Pinto Mancera</t>
+  </si>
+  <si>
+    <t>Alfredo De La Peña, Cra 7 Cl 15#50</t>
+  </si>
+  <si>
+    <t>efrainpintomancera@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -429,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,6 +603,23 @@
       </c>
       <c r="E9">
         <v>54527415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10">
+        <v>8541524514</v>
       </c>
     </row>
   </sheetData>
@@ -604,6 +633,7 @@
     <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="D8" r:id="rId7" xr:uid="{5F4A3C88-33F1-4B38-BF59-1C1BE1587A56}"/>
     <hyperlink ref="D9" r:id="rId8" xr:uid="{B1536EE0-163E-4A4D-9F85-56DCF9FFCA47}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{9343392A-9FE0-4D42-A590-33CFFF28936B}"/>
   </hyperlinks>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>